<commit_message>
Conexao com DB, Insercao de dados nas tabelas
</commit_message>
<xml_diff>
--- a/Plano Projeto.xlsx
+++ b/Plano Projeto.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Desktop\Programação\Teste Junior\Projeto Inicio Dev Junior\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programas\wamp64\www\notven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6862BEC-1CFF-46F6-A82C-0CDEBD134B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDBD079-7C00-4EAC-9287-3567BC88AFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
   <si>
     <t>O projeto é um site de notícias e vendas(simples).</t>
   </si>
@@ -248,6 +248,36 @@
   </si>
   <si>
     <t>tabelas</t>
+  </si>
+  <si>
+    <t>responsivo</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>7º</t>
+  </si>
+  <si>
+    <t>8º</t>
+  </si>
+  <si>
+    <t>Site dinâmico</t>
+  </si>
+  <si>
+    <t>conf. Search</t>
+  </si>
+  <si>
+    <t>9º</t>
+  </si>
+  <si>
+    <t>10º</t>
+  </si>
+  <si>
+    <t>Paginas</t>
+  </si>
+  <si>
+    <t>métodos PDO</t>
   </si>
 </sst>
 </file>
@@ -519,54 +549,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -851,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,21 +1008,21 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="17" t="s">
+      <c r="F15" s="20"/>
+      <c r="G15" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="H15" s="23"/>
-      <c r="I15" s="18"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="20"/>
       <c r="K15" s="3"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
@@ -1006,11 +1036,14 @@
       <c r="B16" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="20"/>
+      <c r="C16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="22"/>
       <c r="K16" s="6"/>
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
@@ -1024,11 +1057,14 @@
       <c r="B17" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="30"/>
-      <c r="G17" s="31"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="33"/>
       <c r="H17" s="15"/>
       <c r="I17" s="16" t="s">
         <v>30</v>
@@ -1046,17 +1082,20 @@
       <c r="B18" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="21" t="s">
+      <c r="F18" s="20"/>
+      <c r="G18" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="H18" s="21" t="s">
+      <c r="H18" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="I18" s="21" t="s">
+      <c r="I18" s="23" t="s">
         <v>34</v>
       </c>
       <c r="K18" s="3"/>
@@ -1072,11 +1111,14 @@
       <c r="B19" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="24"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="26"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
       <c r="K19" s="12"/>
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
@@ -1090,11 +1132,14 @@
       <c r="B20" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="21"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
       <c r="K20" s="12"/>
       <c r="L20" s="13"/>
       <c r="M20" s="13"/>
@@ -1105,13 +1150,19 @@
       <c r="A21" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="17" t="s">
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="23"/>
+      <c r="F21" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="23"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="21"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="23"/>
       <c r="K21" s="12"/>
       <c r="L21" s="13"/>
       <c r="M21" s="13"/>
@@ -1119,11 +1170,20 @@
       <c r="O21" s="14"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E22" s="28"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="28"/>
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="30"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="30"/>
       <c r="K22" s="12"/>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
@@ -1131,11 +1191,17 @@
       <c r="O22" s="14"/>
     </row>
     <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="22"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="22"/>
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="24"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="24"/>
       <c r="K23" s="12"/>
       <c r="L23" s="13"/>
       <c r="M23" s="13"/>
@@ -1143,19 +1209,25 @@
       <c r="O23" s="14"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E24" s="21" t="s">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="21" t="s">
+      <c r="F24" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G24" s="21" t="s">
+      <c r="G24" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H24" s="21" t="s">
+      <c r="H24" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="I24" s="21" t="s">
+      <c r="I24" s="23" t="s">
         <v>40</v>
       </c>
       <c r="K24" s="12"/>
@@ -1165,11 +1237,17 @@
       <c r="O24" s="14"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
       <c r="K25" s="12"/>
       <c r="L25" s="13"/>
       <c r="M25" s="13"/>
@@ -1177,11 +1255,11 @@
       <c r="O25" s="14"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
       <c r="K26" s="6"/>
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
@@ -1189,15 +1267,15 @@
       <c r="O26" s="8"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="18"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="17" t="s">
+      <c r="F27" s="20"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="I27" s="18"/>
+      <c r="I27" s="20"/>
       <c r="K27" s="3"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
@@ -1205,11 +1283,11 @@
       <c r="O27" s="5"/>
     </row>
     <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E28" s="19"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="20"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="22"/>
       <c r="K28" s="6"/>
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>

</xml_diff>

<commit_message>
Paginas mercado e noticias
</commit_message>
<xml_diff>
--- a/Plano Projeto.xlsx
+++ b/Plano Projeto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programas\wamp64\www\notven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDBD079-7C00-4EAC-9287-3567BC88AFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64335B55-F583-48F6-9AC5-B7586C2B4858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
   <si>
     <t>O projeto é um site de notícias e vendas(simples).</t>
   </si>
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t>3-4 campos</t>
-  </si>
-  <si>
-    <t>carousel</t>
   </si>
   <si>
     <t>clicável</t>
@@ -565,37 +562,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -882,7 +879,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,21 +930,21 @@
         <v>6</v>
       </c>
       <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
         <v>24</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>25</v>
-      </c>
-      <c r="H6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -955,24 +952,21 @@
       <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -980,48 +974,45 @@
       <c r="D9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>21</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>22</v>
-      </c>
-      <c r="D12" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F15" s="20"/>
       <c r="G15" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" s="25"/>
+        <v>27</v>
+      </c>
+      <c r="H15" s="23"/>
       <c r="I15" s="20"/>
       <c r="K15" s="3"/>
       <c r="L15" s="4"/>
@@ -1031,18 +1022,18 @@
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E16" s="21"/>
       <c r="F16" s="22"/>
       <c r="G16" s="21"/>
-      <c r="H16" s="29"/>
+      <c r="H16" s="24"/>
       <c r="I16" s="22"/>
       <c r="K16" s="6"/>
       <c r="L16" s="7"/>
@@ -1052,22 +1043,22 @@
     </row>
     <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="32"/>
-      <c r="G17" s="33"/>
+        <v>55</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="26"/>
+      <c r="G17" s="27"/>
       <c r="H17" s="15"/>
       <c r="I17" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K17" s="9"/>
       <c r="L17" s="10"/>
@@ -1077,26 +1068,26 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E18" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="20"/>
+      <c r="G18" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="20"/>
-      <c r="G18" s="23" t="s">
+      <c r="H18" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="H18" s="23" t="s">
+      <c r="I18" s="30" t="s">
         <v>33</v>
-      </c>
-      <c r="I18" s="23" t="s">
-        <v>34</v>
       </c>
       <c r="K18" s="3"/>
       <c r="L18" s="4"/>
@@ -1106,19 +1097,19 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
+        <v>55</v>
+      </c>
+      <c r="E19" s="28"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
       <c r="K19" s="12"/>
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
@@ -1127,19 +1118,19 @@
     </row>
     <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E20" s="21"/>
       <c r="F20" s="22"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
       <c r="K20" s="12"/>
       <c r="L20" s="13"/>
       <c r="M20" s="13"/>
@@ -1148,21 +1139,21 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
         <v>55</v>
       </c>
-      <c r="C21" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" s="23"/>
+      <c r="E21" s="30"/>
       <c r="F21" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" s="25"/>
+        <v>34</v>
+      </c>
+      <c r="G21" s="23"/>
       <c r="H21" s="20"/>
-      <c r="I21" s="23"/>
+      <c r="I21" s="30"/>
       <c r="K21" s="12"/>
       <c r="L21" s="13"/>
       <c r="M21" s="13"/>
@@ -1171,19 +1162,19 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="30"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="30"/>
+        <v>55</v>
+      </c>
+      <c r="E22" s="31"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="31"/>
       <c r="K22" s="12"/>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
@@ -1192,16 +1183,19 @@
     </row>
     <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E23" s="24"/>
+        <v>62</v>
+      </c>
+      <c r="C23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="32"/>
       <c r="F23" s="21"/>
-      <c r="G23" s="29"/>
+      <c r="G23" s="24"/>
       <c r="H23" s="22"/>
-      <c r="I23" s="24"/>
+      <c r="I23" s="32"/>
       <c r="K23" s="12"/>
       <c r="L23" s="13"/>
       <c r="M23" s="13"/>
@@ -1210,25 +1204,25 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="23" t="s">
+      <c r="G24" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="G24" s="23" t="s">
+      <c r="H24" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="H24" s="23" t="s">
+      <c r="I24" s="30" t="s">
         <v>39</v>
-      </c>
-      <c r="I24" s="23" t="s">
-        <v>40</v>
       </c>
       <c r="K24" s="12"/>
       <c r="L24" s="13"/>
@@ -1238,16 +1232,16 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="30"/>
+        <v>58</v>
+      </c>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
       <c r="K25" s="12"/>
       <c r="L25" s="13"/>
       <c r="M25" s="13"/>
@@ -1255,11 +1249,11 @@
       <c r="O25" s="14"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
       <c r="K26" s="6"/>
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
@@ -1268,12 +1262,12 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E27" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F27" s="20"/>
-      <c r="G27" s="23"/>
+      <c r="G27" s="30"/>
       <c r="H27" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I27" s="20"/>
       <c r="K27" s="3"/>
@@ -1285,7 +1279,7 @@
     <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E28" s="21"/>
       <c r="F28" s="22"/>
-      <c r="G28" s="24"/>
+      <c r="G28" s="32"/>
       <c r="H28" s="21"/>
       <c r="I28" s="22"/>
       <c r="K28" s="6"/>
@@ -1296,13 +1290,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="E15:F16"/>
-    <mergeCell ref="G15:I16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E18:F20"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="I18:I20"/>
     <mergeCell ref="E27:F28"/>
     <mergeCell ref="H27:I28"/>
     <mergeCell ref="G27:G28"/>
@@ -1314,6 +1301,13 @@
     <mergeCell ref="I24:I26"/>
     <mergeCell ref="E21:E23"/>
     <mergeCell ref="I21:I23"/>
+    <mergeCell ref="E15:F16"/>
+    <mergeCell ref="G15:I16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E18:F20"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="I18:I20"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>

</xml_diff>